<commit_message>
Excel toimii kuin unelma
</commit_message>
<xml_diff>
--- a/Project_Notebook.xlsx
+++ b/Project_Notebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\GitHub\Studio\Studio\UiPath.Studio.Plugin.Workflow\ProjectTemplates\Business Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e919eb1f4aac589/Tiedostot/UiPath/Digi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841250D0-30A1-4773-B3A3-B7E3E0F9044F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841250D0-30A1-4773-B3A3-B7E3E0F9044F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="18700" windowHeight="9580" activeTab="5" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="9510" yWindow="-1200" windowWidth="19380" windowHeight="10260" activeTab="5" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
@@ -353,13 +353,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="6">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="###,000"/>
-    <numFmt numFmtId="165" formatCode="yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="dd\-mmm"/>
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="###,000"/>
+    <numFmt numFmtId="168" formatCode="yyyy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -747,7 +746,7 @@
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFill="0" applyBorder="0">
       <alignment wrapText="1"/>
     </xf>
@@ -767,7 +766,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="5" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1" indent="4"/>
     </xf>
@@ -780,14 +779,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
-    <xf numFmtId="6" fontId="1" fillId="5" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" applyNumberFormat="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="11"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
@@ -803,28 +802,27 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="16" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="5" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="5" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -835,42 +833,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
@@ -885,7 +864,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -895,10 +873,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1491,10 +1469,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7265625" customWidth="1"/>
-    <col min="2" max="2" width="23.54296875" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1505,311 +1483,293 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53392D88-1157-4343-9701-AA198E0565D5}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.54296875" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" customWidth="1"/>
-    <col min="3" max="4" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-    </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+    </row>
+    <row r="2" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="2">
         <f ca="1">TODAY()</f>
-        <v>44097</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="25" t="s">
+        <v>45008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="43" t="str">
+      <c r="B8" s="28" t="str">
         <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
-        <v>2020-09-30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="25" t="s">
+        <v>2023-03-30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="43" t="str">
+      <c r="B9" s="28" t="str">
         <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
-        <v>2020-10-02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2023-04-03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="44" t="str">
+      <c r="B10" s="29" t="str">
         <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
-        <v>20200923</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20230323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="43" t="str">
+      <c r="B12" s="28" t="str">
         <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
-        <v>2020-09-23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2023-03-23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="43" t="str">
+      <c r="B13" s="28" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-6, preferred_date_format)</f>
-        <v>2020-09-14</v>
-      </c>
-      <c r="C13" s="43" t="str">
+        <v>2023-03-13</v>
+      </c>
+      <c r="C13" s="28" t="str">
         <f ca="1">TEXT(LastWeekMonday+4, preferred_date_format)</f>
-        <v>2020-09-18</v>
-      </c>
-      <c r="D13" s="45" t="str">
+        <v>2023-03-17</v>
+      </c>
+      <c r="D13" s="30" t="str">
         <f ca="1">TEXT(LastWeekFriday+2, preferred_date_format)</f>
-        <v>2020-09-20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2023-03-19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="43" t="str">
+      <c r="B14" s="28" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1), preferred_date_format)</f>
-        <v>2020-08-01</v>
-      </c>
-      <c r="C14" s="43" t="str">
+        <v>2023-02-01</v>
+      </c>
+      <c r="C14" s="28" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), 0), preferred_date_format)</f>
-        <v>2020-08-31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2023-02-28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="43" t="str">
+      <c r="B15" s="28" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY()),1)-1,1), preferred_date_format)</f>
-        <v>2020-09-01</v>
-      </c>
-      <c r="C15" s="43" t="str">
+        <v>2023-03-01</v>
+      </c>
+      <c r="C15" s="28" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),-1), preferred_date_format)</f>
-        <v>2020-09-30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="49" t="s">
+        <v>2023-03-31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="6" t="str">
+      <c r="B23" t="str">
         <f>LEFT(B19, FIND(B20, B19)-1)</f>
         <v>2008</v>
       </c>
-      <c r="C23" s="6" t="str">
+      <c r="C23" t="str">
         <f>RIGHT(B19, LEN(B19)-LEN(B23)-1)</f>
         <v>12月31日 (水)</v>
       </c>
-      <c r="D23" s="7" t="str">
+      <c r="D23" s="6" t="str">
         <f>IF(D20&lt;&gt;"", LEFT(C23, FIND(D20, C23)-1), C23)</f>
         <v>12月31</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="13" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="6" t="str">
+      <c r="B24" t="str">
         <f>LEFT(C23, FIND(C20, C23)-1)</f>
         <v>12</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="13" t="s">
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="6" t="str">
+      <c r="B25" t="str">
         <f>RIGHT(D23, LEN(D23)-LEN(B24)-1)</f>
         <v>31</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="6" t="str">
+      <c r="B26" t="str">
         <f>IF(FIND("Y", B21) = 1, B23, IF(FIND("Y", B21) = 2, B24, B25))</f>
         <v>2008</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
+      <c r="D26" s="6"/>
       <c r="F26">
         <f>FIND("Y", B21)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="6" t="str">
+      <c r="B27" t="str">
         <f>IF(FIND("M", B21) = 1, B23, IF(FIND("M", B21) = 2, B24, B25))</f>
         <v>12</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="6" t="str">
+      <c r="B28" t="str">
         <f>IF(FIND("D", B21) = 1, B23, IF(FIND("D", B21) = 2, B24, B25))</f>
         <v>31</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="14" t="s">
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="46" t="s">
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="6" t="str">
+      <c r="B30" t="str">
         <f>preferred_date_format</f>
         <v>yyyy-mm-dd</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="26"/>
-    </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="15" t="s">
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="8" t="str">
+      <c r="B31" s="7" t="str">
         <f>TEXT(DATE(B26, B27, B28), B30)</f>
         <v>2008-12-31</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1831,40 +1791,40 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="25" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="18" t="s">
         <v>65</v>
       </c>
       <c r="C4" t="s">
@@ -1880,7 +1840,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1891,18 +1851,18 @@
       <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="28" t="str">
+      <c r="F5" s="17" t="str">
         <f>TRIM(MID(Text_Input, FIND(D5,Text_Input)+LEN(D5), IFERROR(FIND(IF(E5="",CHAR(10),E5),Text_Input,FIND(D5,Text_Input)+LEN(D5)),LEN(Text_Input)+1)-FIND(D5,Text_Input)-LEN(D5)))</f>
         <v>C.</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1913,16 +1873,15 @@
       <c r="C6" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="28" t="str">
+      <c r="F6" s="17" t="str">
         <f>TRIM(MID(Text_Input, FIND(D6,Text_Input)+LEN(D6), IFERROR(FIND(IF(E6="",CHAR(10),E6),Text_Input,FIND(D6,Text_Input)+LEN(D6)),LEN(Text_Input)+1)-FIND(D6,Text_Input)-LEN(D6)))</f>
         <v>C. Doe</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1933,16 +1892,15 @@
       <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25" t="s">
+      <c r="E7" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="28" t="str">
+      <c r="F7" s="17" t="str">
         <f>TRIM(MID(Text_Input, FIND(D7,Text_Input)+LEN(D7), IFERROR(FIND(IF(E7="",CHAR(10),E7),Text_Input,FIND(D7,Text_Input)+LEN(D7)),LEN(Text_Input)+1)-FIND(D7,Text_Input)-LEN(D7)))</f>
         <v>John C.</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1953,25 +1911,24 @@
       <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="28" t="str">
+      <c r="F8" s="17" t="str">
         <f>TRIM(MID(Text_Input, FIND(D8,Text_Input)+LEN(D8), IFERROR(FIND(IF(E8="",CHAR(10),E8),Text_Input,FIND(D8,Text_Input)+LEN(D8)),LEN(Text_Input)+1)-FIND(D8,Text_Input)-LEN(D8)))</f>
         <v>Doe</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="28" t="str">
+      <c r="F9" s="17" t="str">
         <f>TRIM(MID(Text_Input, FIND(D9,Text_Input)+LEN(D9), IFERROR(FIND(IF(E9="",CHAR(10),E9),Text_Input,FIND(D9,Text_Input)+LEN(D9)),LEN(Text_Input)+1)-FIND(D9,Text_Input)-LEN(D9)))</f>
         <v>John C. Doe</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1982,7 +1939,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1993,7 +1950,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2005,7 +1962,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2017,12 +1974,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2034,7 +1991,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -2046,7 +2003,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>64</v>
       </c>
@@ -2069,54 +2026,54 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-    </row>
-    <row r="3" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="38"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="18">
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5">
         <f>VALUE(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Number_Input, CHAR(13), ""), CHAR(10), ""), CHAR(160), "")))</f>
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2125,7 +2082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -2134,55 +2091,55 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="49" t="s">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="51"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="B9" s="36"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="7"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="15" t="s">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <f>IF(B12&lt;&gt;"",IF(B13&lt;&gt;"",_xlfn.NUMBERVALUE(B11, B12, B13),_xlfn.NUMBERVALUE(B11, B12)),IF(B13&lt;&gt;"",_xlfn.NUMBERVALUE(B11,, B13),_xlfn.NUMBERVALUE(B11)))</f>
         <v>123456.78</v>
       </c>
@@ -2206,102 +2163,102 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="4" width="15.1796875" customWidth="1"/>
+    <col min="3" max="4" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-    </row>
-    <row r="3" spans="1:4" s="42" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="49" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="51"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="27" t="s">
+      <c r="B4" s="36"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="26"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="17"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="23" t="s">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="17" t="str">
+      <c r="B8" s="6" t="str">
         <f>TRIM(RIGHT(SUBSTITUTE(B6,"\",REPT(" ",LEN(B6))),LEN(B6)))</f>
         <v>Untitled Document.docx</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="17" t="str">
+      <c r="B9" s="6" t="str">
         <f>TRIM(RIGHT(SUBSTITUTE(B8,".",REPT(" ",LEN(B8))),LEN(B8)))</f>
         <v>docx</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="17" t="str">
+      <c r="B10" s="6" t="str">
         <f>LEFT(B8, LEN(B8)-LEN(B9)-1)</f>
         <v>Untitled Document</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="18" t="str">
+      <c r="B11" s="9" t="str">
         <f>LEFT(B6, LEN(B6)-LEN(B8))</f>
         <v>C:\temp\</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="25" t="str">
+      <c r="B15" t="str">
         <f>FileNameNoExtension &amp; "." &amp; FileExtension</f>
         <v>Untitled Document.docx</v>
       </c>
@@ -2320,119 +2277,117 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88115396-113A-4E92-ABEE-648E1977C738}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="165.54296875" style="30" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="30"/>
+    <col min="1" max="1" width="165.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36"/>
-    </row>
-    <row r="2" spans="1:5" ht="35" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22"/>
+    </row>
+    <row r="2" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="37" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="35"/>
-      <c r="D4" s="31"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="34" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="33"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="35"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="35"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="35"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="35"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="35"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="35"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="35"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="35"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="35"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="35"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="35"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="35"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="35"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="35"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="35"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="34" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="37" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="37" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="37" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="37" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nyt toimii siihen asti että hakee 20 ostolaskua jotka maksettava
</commit_message>
<xml_diff>
--- a/Project_Notebook.xlsx
+++ b/Project_Notebook.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841250D0-30A1-4773-B3A3-B7E3E0F9044F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="-1200" windowWidth="19380" windowHeight="10260" activeTab="5" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="9730" yWindow="-980" windowWidth="17945" windowHeight="9505" activeTab="5" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B4" s="2">
         <f ca="1">TODAY()</f>
-        <v>45008</v>
+        <v>45009</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B8" s="28" t="str">
         <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
-        <v>2023-03-30</v>
+        <v>2023-03-31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="B9" s="28" t="str">
         <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
-        <v>2023-04-03</v>
+        <v>2023-04-04</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="B10" s="29" t="str">
         <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
-        <v>20230323</v>
+        <v>20230324</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B12" s="28" t="str">
         <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
-        <v>2023-03-23</v>
+        <v>2023-03-24</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>